<commit_message>
Update report table functionality
When inserting the complete report file into the "report" table, there was an error with the `update_date` format. This code now handles different date formatting, specifically whether the date ends with the complete 4-digit year format (i.e. "/2022") and not the standard 2-digit year format (i.e. "/22").
</commit_message>
<xml_diff>
--- a/sss/data/report_data/Year_Type_SSS_CPI month year_20220715_DBu.xlsx
+++ b/sss/data/report_data/Year_Type_SSS_CPI month year_20220715_DBu.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hec20/SSS/sss/data/report_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A77B47-A95F-F349-99D4-A3190CE2AC0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497036C9-5FD2-C340-B330-947840B60E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="15380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="15320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$8</definedName>
-    <definedName name="Z_00CB0BAB_A7CD_4522_9599_5EF0CAC2BF84_.wvu.FilterData" localSheetId="0" hidden="1">Sheet1!$A$1:$K$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$9</definedName>
+    <definedName name="Z_00CB0BAB_A7CD_4522_9599_5EF0CAC2BF84_.wvu.FilterData" localSheetId="0" hidden="1">Sheet1!$A$1:$K$9</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <customWorkbookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>Year</t>
   </si>
@@ -120,13 +120,19 @@
   </si>
   <si>
     <t>Novembre</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>Aku 06/21/2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,11 +144,20 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -193,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -201,6 +216,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J407"/>
+  <dimension ref="A1:K408"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -437,7 +454,7 @@
     <col min="12" max="30" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -464,7 +481,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>2018</v>
       </c>
@@ -487,7 +504,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2018</v>
       </c>
@@ -514,7 +531,7 @@
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2018</v>
       </c>
@@ -540,101 +557,127 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+    <row r="5" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>2018</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="6">
+        <v>2017</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
         <v>2019</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="3">
-        <v>2019</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="J5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>2022</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="3">
-        <v>2022</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>14</v>
+        <v>2019</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="J6" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>2022</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2022</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E8" s="3">
         <v>2021</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <v>2020</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="3">
-        <v>2019</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="2" t="s">
+    </row>
+    <row r="9" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>2020</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="3">
+        <v>2019</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1026,12 +1069,13 @@
     <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A1:F8" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:F9" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <customSheetViews>
     <customSheetView guid="{00CB0BAB-A7CD-4522-9599-5EF0CAC2BF84}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:K1001" xr:uid="{3DCD12E0-B076-BB4C-942D-0F409FD0A0A3}"/>
+      <autoFilter ref="A1:K1001" xr:uid="{18A706AC-EF42-CB45-8CF9-EEE90AEDB7FD}"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Update report table functionality (#52)
When inserting the complete report file into the "report" table, there was an error with the `update_date` format. This code now handles different date formatting, specifically whether the date ends with the complete 4-digit year format (i.e. "/2022") and not the standard 2-digit year format (i.e. "/22").

Co-authored-by: Hector Sosa <hec20@Hectors-MacBook-Pro.local>
</commit_message>
<xml_diff>
--- a/sss/data/report_data/Year_Type_SSS_CPI month year_20220715_DBu.xlsx
+++ b/sss/data/report_data/Year_Type_SSS_CPI month year_20220715_DBu.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hec20/SSS/sss/data/report_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A77B47-A95F-F349-99D4-A3190CE2AC0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497036C9-5FD2-C340-B330-947840B60E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="15380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="15320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$8</definedName>
-    <definedName name="Z_00CB0BAB_A7CD_4522_9599_5EF0CAC2BF84_.wvu.FilterData" localSheetId="0" hidden="1">Sheet1!$A$1:$K$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$9</definedName>
+    <definedName name="Z_00CB0BAB_A7CD_4522_9599_5EF0CAC2BF84_.wvu.FilterData" localSheetId="0" hidden="1">Sheet1!$A$1:$K$9</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <customWorkbookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>Year</t>
   </si>
@@ -120,13 +120,19 @@
   </si>
   <si>
     <t>Novembre</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>Aku 06/21/2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,11 +144,20 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -193,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -201,6 +216,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J407"/>
+  <dimension ref="A1:K408"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -437,7 +454,7 @@
     <col min="12" max="30" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -464,7 +481,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>2018</v>
       </c>
@@ -487,7 +504,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2018</v>
       </c>
@@ -514,7 +531,7 @@
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2018</v>
       </c>
@@ -540,101 +557,127 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+    <row r="5" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>2018</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="6">
+        <v>2017</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
         <v>2019</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="3">
-        <v>2019</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="J5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>2022</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="3">
-        <v>2022</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>14</v>
+        <v>2019</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="J6" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>2022</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2022</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E8" s="3">
         <v>2021</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <v>2020</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="3">
-        <v>2019</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="2" t="s">
+    </row>
+    <row r="9" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>2020</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="3">
+        <v>2019</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1026,12 +1069,13 @@
     <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A1:F8" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:F9" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <customSheetViews>
     <customSheetView guid="{00CB0BAB-A7CD-4522-9599-5EF0CAC2BF84}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:K1001" xr:uid="{3DCD12E0-B076-BB4C-942D-0F409FD0A0A3}"/>
+      <autoFilter ref="A1:K1001" xr:uid="{18A706AC-EF42-CB45-8CF9-EEE90AEDB7FD}"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>